<commit_message>
First addition of 033 R Markdown
</commit_message>
<xml_diff>
--- a/_site/files/schedule_modules.xlsx
+++ b/_site/files/schedule_modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/dataviz-site/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="14_{322453E6-7958-7F45-A2A8-EC9083DB3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8F347EE-678B-5542-8861-0379DD0AFA96}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="14_{322453E6-7958-7F45-A2A8-EC9083DB3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEBC4588-0AD3-0E41-9079-EEC824AEDDDB}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16300" activeTab="1" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
   <si>
     <t>Principles of data visualization</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Topic</t>
+  </si>
+  <si>
+    <t>2: Coding fundamentals</t>
   </si>
 </sst>
 </file>
@@ -637,7 +640,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,7 +699,7 @@
         <v>44810</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -710,7 +713,7 @@
         <v>44817</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -724,7 +727,7 @@
         <v>44825</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Updating R Markdown, starting ggplot
</commit_message>
<xml_diff>
--- a/_site/files/schedule_modules.xlsx
+++ b/_site/files/schedule_modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/dataviz-site/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="14_{322453E6-7958-7F45-A2A8-EC9083DB3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEBC4588-0AD3-0E41-9079-EEC824AEDDDB}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="14_{322453E6-7958-7F45-A2A8-EC9083DB3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92469CCE-4023-B34B-B5F2-4C9700C93277}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16300" activeTab="1" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
+    <workbookView xWindow="14880" yWindow="5200" windowWidth="28040" windowHeight="16300" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
   <si>
     <t>Principles of data visualization</t>
   </si>
@@ -47,12 +47,6 @@
     <t>R Markdown for reproducible research</t>
   </si>
   <si>
-    <t>Grammar of graphics</t>
-  </si>
-  <si>
-    <t>Themes, labels, facets</t>
-  </si>
-  <si>
     <t>Data distributions</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>1: Principles</t>
   </si>
   <si>
-    <t>2: Coding fundamental</t>
-  </si>
-  <si>
     <t>3: Data exploration</t>
   </si>
   <si>
@@ -102,6 +93,12 @@
   </si>
   <si>
     <t>2: Coding fundamentals</t>
+  </si>
+  <si>
+    <t>ggplot 101</t>
+  </si>
+  <si>
+    <t>Themes, labels, facets (ggplot 102)</t>
   </si>
 </sst>
 </file>
@@ -456,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F342C0D-B564-AC4C-B9F2-1430BA1BF96D}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,13 +464,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -481,7 +478,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -492,7 +489,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -503,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -514,10 +511,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -525,10 +522,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -536,10 +533,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,10 +544,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -558,10 +555,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -569,10 +566,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,10 +577,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -591,10 +588,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -602,10 +599,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -613,10 +610,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,10 +621,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -639,28 +636,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AC0B77-377C-2E43-B142-D9BC271E0496}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -671,7 +668,7 @@
         <v>44796</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -685,7 +682,7 @@
         <v>44803</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -699,7 +696,7 @@
         <v>44810</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -713,10 +710,10 @@
         <v>44817</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -727,10 +724,10 @@
         <v>44825</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -741,10 +738,10 @@
         <v>44832</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -755,10 +752,10 @@
         <v>44838</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -769,10 +766,10 @@
         <v>44845</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,10 +780,10 @@
         <v>44852</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -797,10 +794,10 @@
         <v>44859</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -811,10 +808,10 @@
         <v>44866</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -825,10 +822,10 @@
         <v>44873</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -839,10 +836,10 @@
         <v>44880</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -853,10 +850,10 @@
         <v>44887</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Module 2 solutions and 07_correlations recitation solutions
</commit_message>
<xml_diff>
--- a/_site/files/schedule_modules.xlsx
+++ b/_site/files/schedule_modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/dataviz-site/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="14_{322453E6-7958-7F45-A2A8-EC9083DB3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92469CCE-4023-B34B-B5F2-4C9700C93277}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="14_{322453E6-7958-7F45-A2A8-EC9083DB3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAB292A6-A95F-C947-AA39-ED4C7E9E2CF9}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="5200" windowWidth="28040" windowHeight="16300" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="22">
   <si>
     <t>Principles of data visualization</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Themes, labels, facets (ggplot 102)</t>
+  </si>
+  <si>
+    <t>Open session, capstone prep</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F342C0D-B564-AC4C-B9F2-1430BA1BF96D}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,10 +558,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -566,10 +566,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -580,7 +580,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -591,7 +591,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -602,7 +602,7 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -613,7 +613,7 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -624,6 +624,17 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add module 3 solutions, 10 manhattan plot recitation solutions, update syllabus to include dates
</commit_message>
<xml_diff>
--- a/_site/files/schedule_modules.xlsx
+++ b/_site/files/schedule_modules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/dataviz-site/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicacooperstone/OneDrive - The Ohio State University/BuckeyeBox Data/JLC_Files/OSU/teaching/data-viz/dataviz-site/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="14_{322453E6-7958-7F45-A2A8-EC9083DB3676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41530C99-CD23-AA48-8F4C-1A20EC680845}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C40CE6C-DF63-484C-A234-8A007B7633E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14120" yWindow="3580" windowWidth="28800" windowHeight="16360" xr2:uid="{21EBE61F-A4F0-3D45-865A-9EB87E85AA6A}"/>
   </bookViews>
@@ -668,7 +668,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D17"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>